<commit_message>
Corrections dossiers + régen
</commit_message>
<xml_diff>
--- a/1-Documentations/5 - Tests/2 - Fiches de tests.xlsx
+++ b/1-Documentations/5 - Tests/2 - Fiches de tests.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Documents\GitHub\LaClemenceDAuguste\1-Documentations\5 - Tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$A$1000</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$A$1000</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="373">
   <si>
     <t>No Fiche</t>
   </si>
@@ -863,9 +868,6 @@
     <t>Demander à envoyer un message sur le chat et chronométrer le temps pris à trouver l'emplacement</t>
   </si>
   <si>
-    <t>II.11</t>
-  </si>
-  <si>
     <t>Animation du plateau de jeu</t>
   </si>
   <si>
@@ -878,9 +880,6 @@
     <t>Tous les déplacements et combats/collisions/tenailles ont bien été traités et animés</t>
   </si>
   <si>
-    <t>II.12</t>
-  </si>
-  <si>
     <t>Affichage des cases valides pour le déplacement</t>
   </si>
   <si>
@@ -893,9 +892,6 @@
     <t>Les cases adjacentes au groupe de pions sont correctement mises en valeur</t>
   </si>
   <si>
-    <t>II.13</t>
-  </si>
-  <si>
     <t>Affichage du plateau complet (tentes, armures, laurier)</t>
   </si>
   <si>
@@ -1110,17 +1106,52 @@
   </si>
   <si>
     <t>Pas de bug, le jeu nous demande de nous reconnecter</t>
+  </si>
+  <si>
+    <t>10min</t>
+  </si>
+  <si>
+    <t>Il devrait être possible de répondre à toute les questions ou du moins de trouver les réponses sur le site de manière rapide</t>
+  </si>
+  <si>
+    <t>5min</t>
+  </si>
+  <si>
+    <t>Il faudrait être capable de configurer une partie avec 4 joueurs et 1 légion par joueur en moins de 5 minutes</t>
+  </si>
+  <si>
+    <t>20sec</t>
+  </si>
+  <si>
+    <t>Il faudrait que le déplacement d'un pion soit intuitif et qu'il ne nécessite pas plus de 20 secondes à être effectué</t>
+  </si>
+  <si>
+    <t>Il faudrait que le fait de passer un tour soit simple à trouver et ne nécessite pas plus de 20 secondes à être effectué</t>
+  </si>
+  <si>
+    <t>30sec</t>
+  </si>
+  <si>
+    <t>Il faudrait que le déplacement du lauriet soit intuitif et qu'il ne nécessite pas plus de 30 secondes à être effectué</t>
+  </si>
+  <si>
+    <t>Il faut que le chat soit visible et intuitif et qu'on ne mette pas plus de 10 secondes à trouver où taper le message qu'on souhaite envoyer</t>
+  </si>
+  <si>
+    <t>II.3</t>
+  </si>
+  <si>
+    <t>II.5</t>
+  </si>
+  <si>
+    <t>II.10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1129,22 +1160,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12.1"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -1172,6 +1188,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1188,14 +1210,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
@@ -1211,93 +1233,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="13">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1356,45 +1333,321 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:Z76"/>
+  <dimension ref="A1:AMK75"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="H52" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
-      <selection pane="topRight" activeCell="I72" activeCellId="0" sqref="I72"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A52" sqref="A52"/>
+      <selection pane="topRight" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.54251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.3076923076923"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="65.4129554655871"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="77.8744939271255"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="125.615384615385"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.97165991902834"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="109.740890688259"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.3846153846154"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="10.0607287449393"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="3.77732793522267"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="1" width="2.12955465587045"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.1417004048583"/>
+    <col min="1" max="1" width="5.5703125" style="1"/>
+    <col min="2" max="2" width="26.5703125" style="1"/>
+    <col min="3" max="3" width="36.28515625" style="1"/>
+    <col min="4" max="4" width="13.85546875" style="1"/>
+    <col min="5" max="5" width="65.42578125" style="1"/>
+    <col min="6" max="6" width="77.85546875" style="1"/>
+    <col min="7" max="7" width="125.5703125" style="1"/>
+    <col min="8" max="8" width="8" style="1"/>
+    <col min="9" max="9" width="109.7109375" style="1"/>
+    <col min="10" max="10" width="12.42578125" style="1"/>
+    <col min="11" max="11" width="10" style="2"/>
+    <col min="12" max="12" width="3.7109375" style="1"/>
+    <col min="13" max="15" width="9.140625" style="1"/>
+    <col min="16" max="17" width="2.140625" style="1"/>
+    <col min="18" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1456,7 +1709,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +1740,7 @@
       <c r="J2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="6" t="n">
+      <c r="K2" s="6">
         <v>41774</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -1496,10 +1749,10 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="7" t="n">
+      <c r="P2" s="7">
         <v>1</v>
       </c>
-      <c r="Q2" s="7" t="n">
+      <c r="Q2" s="7">
         <v>2</v>
       </c>
       <c r="R2" s="8"/>
@@ -1512,7 +1765,7 @@
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>27</v>
       </c>
@@ -1543,7 +1796,7 @@
       <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="6" t="n">
+      <c r="K3" s="6">
         <v>41774</v>
       </c>
       <c r="L3" s="5" t="s">
@@ -1552,10 +1805,10 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="7" t="n">
+      <c r="P3" s="7">
         <v>3</v>
       </c>
-      <c r="Q3" s="7" t="n">
+      <c r="Q3" s="7">
         <v>3</v>
       </c>
       <c r="R3" s="8"/>
@@ -1568,7 +1821,7 @@
       <c r="Y3" s="8"/>
       <c r="Z3" s="8"/>
     </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -1599,7 +1852,7 @@
       <c r="J4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="6" t="n">
+      <c r="K4" s="6">
         <v>41774</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -1608,10 +1861,10 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="7" t="n">
+      <c r="P4" s="7">
         <v>2</v>
       </c>
-      <c r="Q4" s="7" t="n">
+      <c r="Q4" s="7">
         <v>2</v>
       </c>
       <c r="R4" s="8"/>
@@ -1624,7 +1877,7 @@
       <c r="Y4" s="8"/>
       <c r="Z4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -1655,7 +1908,7 @@
       <c r="J5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="6" t="n">
+      <c r="K5" s="6">
         <v>41774</v>
       </c>
       <c r="L5" s="5" t="s">
@@ -1664,10 +1917,10 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="7" t="n">
+      <c r="P5" s="7">
         <v>3</v>
       </c>
-      <c r="Q5" s="7" t="n">
+      <c r="Q5" s="7">
         <v>3</v>
       </c>
       <c r="R5" s="8"/>
@@ -1680,7 +1933,7 @@
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>41</v>
       </c>
@@ -1711,7 +1964,7 @@
       <c r="J6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="6" t="n">
+      <c r="K6" s="6">
         <v>41774</v>
       </c>
       <c r="L6" s="5" t="s">
@@ -1720,10 +1973,10 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="7" t="n">
+      <c r="P6" s="7">
         <v>3</v>
       </c>
-      <c r="Q6" s="7" t="n">
+      <c r="Q6" s="7">
         <v>3</v>
       </c>
       <c r="R6" s="8"/>
@@ -1736,7 +1989,7 @@
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
     </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>44</v>
       </c>
@@ -1770,10 +2023,10 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="7" t="n">
+      <c r="P7" s="7">
         <v>2</v>
       </c>
-      <c r="Q7" s="7" t="n">
+      <c r="Q7" s="7">
         <v>2</v>
       </c>
       <c r="R7" s="8"/>
@@ -1786,7 +2039,7 @@
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
     </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>49</v>
       </c>
@@ -1820,10 +2073,10 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="7" t="n">
+      <c r="P8" s="7">
         <v>3</v>
       </c>
-      <c r="Q8" s="7" t="n">
+      <c r="Q8" s="7">
         <v>3</v>
       </c>
       <c r="R8" s="8"/>
@@ -1836,7 +2089,7 @@
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>53</v>
       </c>
@@ -1870,10 +2123,10 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="7" t="n">
+      <c r="P9" s="7">
         <v>3</v>
       </c>
-      <c r="Q9" s="7" t="n">
+      <c r="Q9" s="7">
         <v>3</v>
       </c>
       <c r="R9" s="8"/>
@@ -1886,7 +2139,7 @@
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>56</v>
       </c>
@@ -1920,10 +2173,10 @@
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="7" t="n">
+      <c r="P10" s="7">
         <v>1</v>
       </c>
-      <c r="Q10" s="7" t="n">
+      <c r="Q10" s="7">
         <v>1</v>
       </c>
       <c r="R10" s="8"/>
@@ -1936,7 +2189,7 @@
       <c r="Y10" s="8"/>
       <c r="Z10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>59</v>
       </c>
@@ -1970,10 +2223,10 @@
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="7" t="n">
+      <c r="P11" s="7">
         <v>3</v>
       </c>
-      <c r="Q11" s="7" t="n">
+      <c r="Q11" s="7">
         <v>3</v>
       </c>
       <c r="R11" s="8"/>
@@ -1986,7 +2239,7 @@
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>64</v>
       </c>
@@ -2020,10 +2273,10 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="7" t="n">
+      <c r="P12" s="7">
         <v>3</v>
       </c>
-      <c r="Q12" s="7" t="n">
+      <c r="Q12" s="7">
         <v>3</v>
       </c>
       <c r="R12" s="8"/>
@@ -2036,7 +2289,7 @@
       <c r="Y12" s="8"/>
       <c r="Z12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>69</v>
       </c>
@@ -2070,10 +2323,10 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="7" t="n">
+      <c r="P13" s="7">
         <v>3</v>
       </c>
-      <c r="Q13" s="7" t="n">
+      <c r="Q13" s="7">
         <v>2</v>
       </c>
       <c r="R13" s="8"/>
@@ -2086,7 +2339,7 @@
       <c r="Y13" s="8"/>
       <c r="Z13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>73</v>
       </c>
@@ -2120,10 +2373,10 @@
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="7" t="n">
+      <c r="P14" s="7">
         <v>2</v>
       </c>
-      <c r="Q14" s="7" t="n">
+      <c r="Q14" s="7">
         <v>2</v>
       </c>
       <c r="R14" s="8"/>
@@ -2136,7 +2389,7 @@
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>78</v>
       </c>
@@ -2170,10 +2423,10 @@
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="7" t="n">
+      <c r="P15" s="7">
         <v>2</v>
       </c>
-      <c r="Q15" s="7" t="n">
+      <c r="Q15" s="7">
         <v>2</v>
       </c>
       <c r="R15" s="8"/>
@@ -2186,7 +2439,7 @@
       <c r="Y15" s="8"/>
       <c r="Z15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>83</v>
       </c>
@@ -2220,10 +2473,10 @@
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
-      <c r="P16" s="12" t="n">
+      <c r="P16" s="12">
         <v>3</v>
       </c>
-      <c r="Q16" s="12" t="n">
+      <c r="Q16" s="12">
         <v>3</v>
       </c>
       <c r="R16" s="8"/>
@@ -2236,7 +2489,7 @@
       <c r="Y16" s="8"/>
       <c r="Z16" s="8"/>
     </row>
-    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>91</v>
       </c>
@@ -2270,10 +2523,10 @@
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="7" t="n">
+      <c r="P17" s="7">
         <v>3</v>
       </c>
-      <c r="Q17" s="7" t="n">
+      <c r="Q17" s="7">
         <v>3</v>
       </c>
       <c r="R17" s="8"/>
@@ -2286,7 +2539,7 @@
       <c r="Y17" s="8"/>
       <c r="Z17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>96</v>
       </c>
@@ -2320,10 +2573,10 @@
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="7" t="n">
+      <c r="P18" s="7">
         <v>3</v>
       </c>
-      <c r="Q18" s="7" t="n">
+      <c r="Q18" s="7">
         <v>3</v>
       </c>
       <c r="R18" s="8"/>
@@ -2336,7 +2589,7 @@
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
     </row>
-    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>102</v>
       </c>
@@ -2370,10 +2623,10 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="7" t="n">
+      <c r="P19" s="7">
         <v>2</v>
       </c>
-      <c r="Q19" s="7" t="n">
+      <c r="Q19" s="7">
         <v>3</v>
       </c>
       <c r="R19" s="8"/>
@@ -2386,7 +2639,7 @@
       <c r="Y19" s="8"/>
       <c r="Z19" s="8"/>
     </row>
-    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>107</v>
       </c>
@@ -2420,10 +2673,10 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="7" t="n">
+      <c r="P20" s="7">
         <v>3</v>
       </c>
-      <c r="Q20" s="7" t="n">
+      <c r="Q20" s="7">
         <v>3</v>
       </c>
       <c r="R20" s="8"/>
@@ -2436,7 +2689,7 @@
       <c r="Y20" s="8"/>
       <c r="Z20" s="8"/>
     </row>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>112</v>
       </c>
@@ -2470,10 +2723,10 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="7" t="n">
+      <c r="P21" s="7">
         <v>3</v>
       </c>
-      <c r="Q21" s="7" t="n">
+      <c r="Q21" s="7">
         <v>3</v>
       </c>
       <c r="R21" s="8"/>
@@ -2486,7 +2739,7 @@
       <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
     </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>119</v>
       </c>
@@ -2520,10 +2773,10 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="7" t="n">
+      <c r="P22" s="7">
         <v>1</v>
       </c>
-      <c r="Q22" s="7" t="n">
+      <c r="Q22" s="7">
         <v>1</v>
       </c>
       <c r="R22" s="8"/>
@@ -2536,7 +2789,7 @@
       <c r="Y22" s="8"/>
       <c r="Z22" s="8"/>
     </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>125</v>
       </c>
@@ -2570,10 +2823,10 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
-      <c r="P23" s="7" t="n">
+      <c r="P23" s="7">
         <v>2</v>
       </c>
-      <c r="Q23" s="7" t="n">
+      <c r="Q23" s="7">
         <v>2</v>
       </c>
       <c r="R23" s="8"/>
@@ -2586,7 +2839,7 @@
       <c r="Y23" s="8"/>
       <c r="Z23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>130</v>
       </c>
@@ -2620,10 +2873,10 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
-      <c r="P24" s="7" t="n">
+      <c r="P24" s="7">
         <v>3</v>
       </c>
-      <c r="Q24" s="7" t="n">
+      <c r="Q24" s="7">
         <v>3</v>
       </c>
       <c r="R24" s="8"/>
@@ -2636,7 +2889,7 @@
       <c r="Y24" s="8"/>
       <c r="Z24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>136</v>
       </c>
@@ -2670,10 +2923,10 @@
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
-      <c r="P25" s="7" t="n">
+      <c r="P25" s="7">
         <v>3</v>
       </c>
-      <c r="Q25" s="7" t="n">
+      <c r="Q25" s="7">
         <v>3</v>
       </c>
       <c r="R25" s="8"/>
@@ -2686,7 +2939,7 @@
       <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>140</v>
       </c>
@@ -2720,10 +2973,10 @@
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
-      <c r="P26" s="7" t="n">
+      <c r="P26" s="7">
         <v>3</v>
       </c>
-      <c r="Q26" s="7" t="n">
+      <c r="Q26" s="7">
         <v>3</v>
       </c>
       <c r="R26" s="8"/>
@@ -2736,7 +2989,7 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>144</v>
       </c>
@@ -2770,10 +3023,10 @@
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
-      <c r="P27" s="7" t="n">
+      <c r="P27" s="7">
         <v>3</v>
       </c>
-      <c r="Q27" s="7" t="n">
+      <c r="Q27" s="7">
         <v>3</v>
       </c>
       <c r="R27" s="8"/>
@@ -2786,7 +3039,7 @@
       <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
     </row>
-    <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>148</v>
       </c>
@@ -2820,10 +3073,10 @@
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
-      <c r="P28" s="7" t="n">
+      <c r="P28" s="7">
         <v>3</v>
       </c>
-      <c r="Q28" s="7" t="n">
+      <c r="Q28" s="7">
         <v>3</v>
       </c>
       <c r="R28" s="8"/>
@@ -2836,7 +3089,7 @@
       <c r="Y28" s="8"/>
       <c r="Z28" s="8"/>
     </row>
-    <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>152</v>
       </c>
@@ -2870,10 +3123,10 @@
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-      <c r="P29" s="7" t="n">
+      <c r="P29" s="7">
         <v>3</v>
       </c>
-      <c r="Q29" s="7" t="n">
+      <c r="Q29" s="7">
         <v>3</v>
       </c>
       <c r="R29" s="8"/>
@@ -2886,7 +3139,7 @@
       <c r="Y29" s="8"/>
       <c r="Z29" s="8"/>
     </row>
-    <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>157</v>
       </c>
@@ -2920,10 +3173,10 @@
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
-      <c r="P30" s="7" t="n">
+      <c r="P30" s="7">
         <v>2</v>
       </c>
-      <c r="Q30" s="7" t="n">
+      <c r="Q30" s="7">
         <v>2</v>
       </c>
       <c r="R30" s="8"/>
@@ -2936,7 +3189,7 @@
       <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>161</v>
       </c>
@@ -2970,10 +3223,10 @@
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
-      <c r="P31" s="7" t="n">
+      <c r="P31" s="7">
         <v>3</v>
       </c>
-      <c r="Q31" s="7" t="n">
+      <c r="Q31" s="7">
         <v>3</v>
       </c>
       <c r="R31" s="8"/>
@@ -2986,7 +3239,7 @@
       <c r="Y31" s="8"/>
       <c r="Z31" s="8"/>
     </row>
-    <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>165</v>
       </c>
@@ -3020,10 +3273,10 @@
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
-      <c r="P32" s="7" t="n">
+      <c r="P32" s="7">
         <v>3</v>
       </c>
-      <c r="Q32" s="7" t="n">
+      <c r="Q32" s="7">
         <v>3</v>
       </c>
       <c r="R32" s="8"/>
@@ -3036,7 +3289,7 @@
       <c r="Y32" s="8"/>
       <c r="Z32" s="8"/>
     </row>
-    <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>169</v>
       </c>
@@ -3067,7 +3320,7 @@
       <c r="J33" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="K33" s="6" t="n">
+      <c r="K33" s="6">
         <v>41781</v>
       </c>
       <c r="L33" s="5" t="s">
@@ -3076,10 +3329,10 @@
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="7" t="n">
+      <c r="P33" s="7">
         <v>2</v>
       </c>
-      <c r="Q33" s="7" t="n">
+      <c r="Q33" s="7">
         <v>2</v>
       </c>
       <c r="R33" s="8"/>
@@ -3092,7 +3345,7 @@
       <c r="Y33" s="8"/>
       <c r="Z33" s="8"/>
     </row>
-    <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>176</v>
       </c>
@@ -3123,7 +3376,7 @@
       <c r="J34" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="K34" s="6" t="n">
+      <c r="K34" s="6">
         <v>41781</v>
       </c>
       <c r="L34" s="5" t="s">
@@ -3132,10 +3385,10 @@
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
-      <c r="P34" s="7" t="n">
+      <c r="P34" s="7">
         <v>2</v>
       </c>
-      <c r="Q34" s="7" t="n">
+      <c r="Q34" s="7">
         <v>2</v>
       </c>
       <c r="R34" s="8"/>
@@ -3148,7 +3401,7 @@
       <c r="Y34" s="8"/>
       <c r="Z34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>179</v>
       </c>
@@ -3179,7 +3432,7 @@
       <c r="J35" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="K35" s="6" t="n">
+      <c r="K35" s="6">
         <v>41781</v>
       </c>
       <c r="L35" s="5" t="s">
@@ -3188,10 +3441,10 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
-      <c r="P35" s="7" t="n">
+      <c r="P35" s="7">
         <v>2</v>
       </c>
-      <c r="Q35" s="7" t="n">
+      <c r="Q35" s="7">
         <v>2</v>
       </c>
       <c r="R35" s="8"/>
@@ -3204,7 +3457,7 @@
       <c r="Y35" s="8"/>
       <c r="Z35" s="8"/>
     </row>
-    <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>184</v>
       </c>
@@ -3238,10 +3491,10 @@
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-      <c r="P36" s="7" t="n">
+      <c r="P36" s="7">
         <v>2</v>
       </c>
-      <c r="Q36" s="7" t="n">
+      <c r="Q36" s="7">
         <v>2</v>
       </c>
       <c r="R36" s="8"/>
@@ -3254,7 +3507,7 @@
       <c r="Y36" s="8"/>
       <c r="Z36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>186</v>
       </c>
@@ -3288,10 +3541,10 @@
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
-      <c r="P37" s="7" t="n">
+      <c r="P37" s="7">
         <v>2</v>
       </c>
-      <c r="Q37" s="7" t="n">
+      <c r="Q37" s="7">
         <v>2</v>
       </c>
       <c r="R37" s="8"/>
@@ -3304,7 +3557,7 @@
       <c r="Y37" s="8"/>
       <c r="Z37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>189</v>
       </c>
@@ -3338,10 +3591,10 @@
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
-      <c r="P38" s="7" t="n">
+      <c r="P38" s="7">
         <v>2</v>
       </c>
-      <c r="Q38" s="7" t="n">
+      <c r="Q38" s="7">
         <v>3</v>
       </c>
       <c r="R38" s="8"/>
@@ -3354,7 +3607,7 @@
       <c r="Y38" s="8"/>
       <c r="Z38" s="8"/>
     </row>
-    <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>197</v>
       </c>
@@ -3388,10 +3641,10 @@
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
-      <c r="P39" s="7" t="n">
+      <c r="P39" s="7">
         <v>1</v>
       </c>
-      <c r="Q39" s="7" t="n">
+      <c r="Q39" s="7">
         <v>1</v>
       </c>
       <c r="R39" s="8"/>
@@ -3404,7 +3657,7 @@
       <c r="Y39" s="8"/>
       <c r="Z39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>201</v>
       </c>
@@ -3438,10 +3691,10 @@
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
-      <c r="P40" s="7" t="n">
+      <c r="P40" s="7">
         <v>2</v>
       </c>
-      <c r="Q40" s="7" t="n">
+      <c r="Q40" s="7">
         <v>3</v>
       </c>
       <c r="R40" s="8"/>
@@ -3454,7 +3707,7 @@
       <c r="Y40" s="8"/>
       <c r="Z40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>205</v>
       </c>
@@ -3488,10 +3741,10 @@
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
       <c r="O41" s="4"/>
-      <c r="P41" s="7" t="n">
+      <c r="P41" s="7">
         <v>2</v>
       </c>
-      <c r="Q41" s="7" t="n">
+      <c r="Q41" s="7">
         <v>2</v>
       </c>
       <c r="R41" s="8"/>
@@ -3504,7 +3757,7 @@
       <c r="Y41" s="8"/>
       <c r="Z41" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>210</v>
       </c>
@@ -3538,10 +3791,10 @@
       <c r="M42" s="4"/>
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
-      <c r="P42" s="7" t="n">
+      <c r="P42" s="7">
         <v>2</v>
       </c>
-      <c r="Q42" s="7" t="n">
+      <c r="Q42" s="7">
         <v>2</v>
       </c>
       <c r="R42" s="8"/>
@@ -3554,7 +3807,7 @@
       <c r="Y42" s="8"/>
       <c r="Z42" s="8"/>
     </row>
-    <row r="43" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>214</v>
       </c>
@@ -3588,10 +3841,10 @@
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
-      <c r="P43" s="7" t="n">
+      <c r="P43" s="7">
         <v>2</v>
       </c>
-      <c r="Q43" s="7" t="n">
+      <c r="Q43" s="7">
         <v>3</v>
       </c>
       <c r="R43" s="8"/>
@@ -3604,7 +3857,7 @@
       <c r="Y43" s="8"/>
       <c r="Z43" s="8"/>
     </row>
-    <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>219</v>
       </c>
@@ -3638,10 +3891,10 @@
       <c r="M44" s="4"/>
       <c r="N44" s="4"/>
       <c r="O44" s="4"/>
-      <c r="P44" s="7" t="n">
+      <c r="P44" s="7">
         <v>2</v>
       </c>
-      <c r="Q44" s="7" t="n">
+      <c r="Q44" s="7">
         <v>1</v>
       </c>
       <c r="R44" s="8"/>
@@ -3654,7 +3907,7 @@
       <c r="Y44" s="8"/>
       <c r="Z44" s="8"/>
     </row>
-    <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>224</v>
       </c>
@@ -3688,10 +3941,10 @@
       <c r="M45" s="4"/>
       <c r="N45" s="4"/>
       <c r="O45" s="4"/>
-      <c r="P45" s="7" t="n">
+      <c r="P45" s="7">
         <v>3</v>
       </c>
-      <c r="Q45" s="7" t="n">
+      <c r="Q45" s="7">
         <v>3</v>
       </c>
       <c r="R45" s="8"/>
@@ -3704,7 +3957,7 @@
       <c r="Y45" s="8"/>
       <c r="Z45" s="8"/>
     </row>
-    <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>229</v>
       </c>
@@ -3738,10 +3991,10 @@
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
-      <c r="P46" s="7" t="n">
+      <c r="P46" s="7">
         <v>2</v>
       </c>
-      <c r="Q46" s="7" t="n">
+      <c r="Q46" s="7">
         <v>3</v>
       </c>
       <c r="R46" s="8"/>
@@ -3754,7 +4007,7 @@
       <c r="Y46" s="8"/>
       <c r="Z46" s="8"/>
     </row>
-    <row r="47" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>232</v>
       </c>
@@ -3788,10 +4041,10 @@
       <c r="M47" s="4"/>
       <c r="N47" s="4"/>
       <c r="O47" s="4"/>
-      <c r="P47" s="7" t="n">
+      <c r="P47" s="7">
         <v>2</v>
       </c>
-      <c r="Q47" s="7" t="n">
+      <c r="Q47" s="7">
         <v>3</v>
       </c>
       <c r="R47" s="8"/>
@@ -3804,7 +4057,7 @@
       <c r="Y47" s="8"/>
       <c r="Z47" s="8"/>
     </row>
-    <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>236</v>
       </c>
@@ -3838,10 +4091,10 @@
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
-      <c r="P48" s="7" t="n">
+      <c r="P48" s="7">
         <v>2</v>
       </c>
-      <c r="Q48" s="7" t="n">
+      <c r="Q48" s="7">
         <v>3</v>
       </c>
       <c r="R48" s="8"/>
@@ -3854,7 +4107,7 @@
       <c r="Y48" s="8"/>
       <c r="Z48" s="8"/>
     </row>
-    <row r="49" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>242</v>
       </c>
@@ -3888,10 +4141,10 @@
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
-      <c r="P49" s="7" t="n">
+      <c r="P49" s="7">
         <v>2</v>
       </c>
-      <c r="Q49" s="7" t="n">
+      <c r="Q49" s="7">
         <v>3</v>
       </c>
       <c r="R49" s="8"/>
@@ -3904,7 +4157,7 @@
       <c r="Y49" s="8"/>
       <c r="Z49" s="8"/>
     </row>
-    <row r="50" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>248</v>
       </c>
@@ -3938,10 +4191,10 @@
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
-      <c r="P50" s="7" t="n">
+      <c r="P50" s="7">
         <v>2</v>
       </c>
-      <c r="Q50" s="7" t="n">
+      <c r="Q50" s="7">
         <v>3</v>
       </c>
       <c r="R50" s="8"/>
@@ -3954,7 +4207,7 @@
       <c r="Y50" s="8"/>
       <c r="Z50" s="8"/>
     </row>
-    <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:26" ht="61.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>253</v>
       </c>
@@ -3976,10 +4229,10 @@
       <c r="G51" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="H51" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="I51" s="13" t="s">
         <v>260</v>
       </c>
       <c r="J51" s="4"/>
@@ -4000,7 +4253,7 @@
       <c r="Y51" s="8"/>
       <c r="Z51" s="8"/>
     </row>
-    <row r="52" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>261</v>
       </c>
@@ -4022,8 +4275,12 @@
       <c r="G52" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
+      <c r="H52" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>361</v>
+      </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -4042,9 +4299,9 @@
       <c r="Y52" s="8"/>
       <c r="Z52" s="8"/>
     </row>
-    <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>265</v>
+        <v>370</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>254</v>
@@ -4064,8 +4321,12 @@
       <c r="G53" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
+      <c r="H53" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>363</v>
+      </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -4084,9 +4345,9 @@
       <c r="Y53" s="8"/>
       <c r="Z53" s="8"/>
     </row>
-    <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>254</v>
@@ -4106,8 +4367,12 @@
       <c r="G54" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
+      <c r="H54" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>365</v>
+      </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -4126,9 +4391,9 @@
       <c r="Y54" s="8"/>
       <c r="Z54" s="8"/>
     </row>
-    <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>271</v>
+        <v>371</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>254</v>
@@ -4148,8 +4413,12 @@
       <c r="G55" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
+      <c r="H55" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>366</v>
+      </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
@@ -4168,9 +4437,9 @@
       <c r="Y55" s="8"/>
       <c r="Z55" s="8"/>
     </row>
-    <row r="56" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>254</v>
@@ -4190,8 +4459,12 @@
       <c r="G56" s="5" t="s">
         <v>276</v>
       </c>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
+      <c r="H56" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>368</v>
+      </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -4210,9 +4483,9 @@
       <c r="Y56" s="8"/>
       <c r="Z56" s="8"/>
     </row>
-    <row r="57" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>254</v>
@@ -4230,8 +4503,12 @@
       <c r="G57" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
+      <c r="H57" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>369</v>
+      </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
@@ -4250,9 +4527,9 @@
       <c r="Y57" s="8"/>
       <c r="Z57" s="8"/>
     </row>
-    <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>254</v>
@@ -4264,19 +4541,19 @@
         <v>85</v>
       </c>
       <c r="E58" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="F58" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="F58" s="5" t="s">
+      <c r="G58" s="5" t="s">
         <v>282</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>283</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>52</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -4296,9 +4573,9 @@
       <c r="Y58" s="8"/>
       <c r="Z58" s="8"/>
     </row>
-    <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>254</v>
@@ -4310,19 +4587,19 @@
         <v>85</v>
       </c>
       <c r="E59" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="G59" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>100</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
@@ -4342,9 +4619,9 @@
       <c r="Y59" s="8"/>
       <c r="Z59" s="8"/>
     </row>
-    <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>290</v>
+        <v>372</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>254</v>
@@ -4356,19 +4633,19 @@
         <v>85</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>66</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>188</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
@@ -4388,33 +4665,33 @@
       <c r="Y60" s="8"/>
       <c r="Z60" s="8"/>
     </row>
-    <row r="61" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -4434,33 +4711,33 @@
       <c r="Y61" s="8"/>
       <c r="Z61" s="8"/>
     </row>
-    <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -4480,33 +4757,33 @@
       <c r="Y62" s="8"/>
       <c r="Z62" s="8"/>
     </row>
-    <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -4526,33 +4803,33 @@
       <c r="Y63" s="8"/>
       <c r="Z63" s="8"/>
     </row>
-    <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>123</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
@@ -4572,33 +4849,33 @@
       <c r="Y64" s="8"/>
       <c r="Z64" s="8"/>
     </row>
-    <row r="65" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>123</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
@@ -4618,33 +4895,33 @@
       <c r="Y65" s="8"/>
       <c r="Z65" s="8"/>
     </row>
-    <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="H66" s="5" t="s">
         <v>123</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
@@ -4664,33 +4941,33 @@
       <c r="Y66" s="8"/>
       <c r="Z66" s="8"/>
     </row>
-    <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>114</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
@@ -4710,33 +4987,33 @@
       <c r="Y67" s="8"/>
       <c r="Z67" s="8"/>
     </row>
-    <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H68" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
@@ -4756,33 +5033,33 @@
       <c r="Y68" s="8"/>
       <c r="Z68" s="8"/>
     </row>
-    <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
@@ -4802,33 +5079,33 @@
       <c r="Y69" s="8"/>
       <c r="Z69" s="8"/>
     </row>
-    <row r="70" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>171</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="H70" s="5" t="s">
         <v>81</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
@@ -4848,33 +5125,33 @@
       <c r="Y70" s="8"/>
       <c r="Z70" s="8"/>
     </row>
-    <row r="71" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D71" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E71" s="11" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="H71" s="11" t="s">
         <v>24</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
@@ -4894,33 +5171,33 @@
       <c r="Y71" s="4"/>
       <c r="Z71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>193</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>123</v>
       </c>
       <c r="I72" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
@@ -4940,33 +5217,33 @@
       <c r="Y72" s="8"/>
       <c r="Z72" s="8"/>
     </row>
-    <row r="73" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F73" s="10" t="s">
         <v>193</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>123</v>
       </c>
       <c r="I73" s="5" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
@@ -4986,33 +5263,33 @@
       <c r="Y73" s="8"/>
       <c r="Z73" s="8"/>
     </row>
-    <row r="74" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="F74" s="10" t="s">
         <v>193</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="H74" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
@@ -5032,33 +5309,33 @@
       <c r="Y74" s="8"/>
       <c r="Z74" s="8"/>
     </row>
-    <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>34</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>24</v>
       </c>
       <c r="I75" s="5" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="J75" s="4"/>
       <c r="K75" s="8"/>
@@ -5078,950 +5355,8 @@
       <c r="Y75" s="8"/>
       <c r="Z75" s="8"/>
     </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="255" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="256" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="257" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="258" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="259" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="260" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="261" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="262" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="263" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="264" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="265" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="266" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="267" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="268" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="269" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="270" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="271" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="272" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="273" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="274" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="275" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="276" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="277" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="278" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="279" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="280" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="281" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="282" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="283" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="284" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="285" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="286" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="287" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="288" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="289" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="290" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="291" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="292" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="293" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="294" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="295" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="296" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="300" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="301" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="302" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="303" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="304" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="305" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="306" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="307" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="308" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="309" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="310" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="311" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="312" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="313" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="314" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="315" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="316" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="317" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="318" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="319" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="320" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="321" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="322" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="323" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="324" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="325" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="326" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="327" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="328" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="329" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="330" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="331" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="332" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="333" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="334" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="335" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="336" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="337" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="338" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="339" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="340" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="341" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="342" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="343" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="344" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="345" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="346" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="347" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="348" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="349" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="350" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="351" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="352" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="353" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="354" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="355" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="356" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="357" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="358" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="359" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="360" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="361" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="362" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="363" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="364" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="365" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="366" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="367" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="368" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="369" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="370" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="371" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="372" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="373" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="374" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="375" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="376" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="377" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="378" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="379" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="380" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="381" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="382" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="383" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="384" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="385" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="386" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="387" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="388" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="389" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="390" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="391" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="392" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="393" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="394" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="395" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="396" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="397" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="398" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="399" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="400" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="401" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="402" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="403" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="404" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="405" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="406" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="407" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="408" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="409" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="410" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="411" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="412" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="413" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="414" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="415" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="416" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="417" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="418" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="419" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="420" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="421" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="422" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="423" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="424" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="425" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="426" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="427" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="428" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="429" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="430" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="431" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="432" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="433" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="434" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="435" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="436" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="437" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="438" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="439" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="440" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="441" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="442" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="443" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="444" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="445" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="446" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="447" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="448" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="449" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="450" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="451" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="452" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="453" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="454" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="455" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="456" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="457" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="458" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="459" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="460" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="461" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="462" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="463" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="464" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="465" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="466" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="467" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="468" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="469" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="470" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="471" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="472" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="473" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="474" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="475" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="478" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="479" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="480" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="481" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="482" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="483" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="484" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="485" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="486" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="487" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="488" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="489" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="490" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="491" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="492" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="493" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="494" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="495" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="496" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="497" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="498" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="499" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="500" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="501" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="502" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="503" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="504" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="505" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="506" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="507" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="508" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="509" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="510" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="511" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="512" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="513" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="514" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="515" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="516" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="517" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="518" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="519" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="520" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="521" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="522" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="523" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="524" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="525" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="526" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="527" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="528" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="529" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="530" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="531" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="532" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="533" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="534" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="535" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="536" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="537" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="538" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="539" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="540" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="541" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="542" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="543" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="544" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="545" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="546" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="547" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="548" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="549" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="550" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="551" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="552" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="553" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="554" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="555" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="556" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="557" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="558" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="559" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="560" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="561" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="562" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="563" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="564" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="565" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="566" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="567" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="568" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="569" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="570" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="571" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="572" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="573" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="574" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="575" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="576" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="577" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="578" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="579" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="580" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="581" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="582" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="583" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="584" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="585" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="586" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="587" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="588" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="589" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="590" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="591" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="592" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="593" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="594" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="595" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="596" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="597" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="598" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="599" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="600" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="601" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="602" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="603" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="604" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="605" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="606" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="607" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="608" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="609" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="610" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="611" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="612" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="613" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="614" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="615" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="616" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="617" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="618" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="619" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="620" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="621" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="622" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="623" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="624" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="625" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="626" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="627" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="628" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="629" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="630" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="631" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="632" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="633" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="634" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="635" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="636" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="637" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="638" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="639" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="640" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="641" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="642" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="643" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="644" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="645" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="646" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="647" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="648" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="649" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="650" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="651" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="652" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="653" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="654" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="655" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="656" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="657" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="658" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="659" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="660" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="661" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="671" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="672" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="673" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="674" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="675" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="676" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="677" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="678" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="679" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="680" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="681" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="682" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="683" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="684" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="690" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="691" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="692" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="693" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="694" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="695" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="696" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="697" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="698" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="699" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="700" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="701" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="702" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="703" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="704" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="705" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="706" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="707" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="708" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="709" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="710" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="711" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="712" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="713" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="714" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="715" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="716" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="717" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="718" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="719" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="720" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="721" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="722" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="723" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="724" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="725" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="726" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="727" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="728" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="729" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="730" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="731" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="732" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="733" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="734" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="735" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="736" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="737" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="738" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="739" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="740" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="741" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="742" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="743" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="744" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="745" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="746" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="747" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="748" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="749" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="750" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="751" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="752" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="753" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="754" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="755" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="756" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="757" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="758" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="759" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="760" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="761" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="762" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="763" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="764" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="765" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="766" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="767" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="768" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="769" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="770" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="771" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="772" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="773" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="774" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="775" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="776" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="777" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="778" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="779" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="780" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="781" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="782" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="783" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="784" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="785" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="786" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="787" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="788" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="789" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="790" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="791" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="792" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="793" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="794" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="795" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="796" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="797" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="798" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="799" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="800" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="801" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="802" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="803" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="804" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="805" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="806" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="807" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="808" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="809" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="810" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="811" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="812" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="813" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="814" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="815" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="816" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="817" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="818" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="819" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="820" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="821" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="822" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="823" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="824" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="825" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="826" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="827" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="828" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="829" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="830" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="831" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="832" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="833" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="834" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="835" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="836" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="837" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="838" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="839" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="841" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="842" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="843" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="844" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="845" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="846" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="847" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="855" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="856" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="857" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="858" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="859" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="867" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="868" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="869" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="870" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="871" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="872" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="876" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="877" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="878" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="879" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="880" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="881" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="882" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="883" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="884" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="885" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="886" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="887" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="888" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="889" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="890" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="891" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="892" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="893" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="894" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="895" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="896" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="897" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="898" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="899" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="900" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="901" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="902" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="903" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="904" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="905" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="906" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="907" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="908" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="909" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="910" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="911" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="912" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="913" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="914" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="915" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="916" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="917" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="918" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="919" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="920" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="921" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="922" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="923" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="924" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="925" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="926" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="927" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="928" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="929" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="930" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="931" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="932" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="933" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="934" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="935" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="936" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="937" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="938" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="939" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="940" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="941" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="942" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="943" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="944" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="945" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="946" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="947" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="948" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="949" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="950" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="951" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="952" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="953" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="954" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="955" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="956" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="957" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="958" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="959" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="960" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="961" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="962" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="963" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="964" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="965" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="966" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="967" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="968" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="969" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="970" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="971" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="972" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="973" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="974" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="975" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="976" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="977" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="978" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="979" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="980" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1004" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1005" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1006" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1009" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1010" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1011" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1012" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>